<commit_message>
variables can be refrenced from sheetname and cellname
</commit_message>
<xml_diff>
--- a/src/excel_wrapper/test/excel_wrapper_test.xlsx
+++ b/src/excel_wrapper/test/excel_wrapper_test.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PLUGIN-1.x\excel_wrapper1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9780"/>
   </bookViews>
@@ -19,12 +24,12 @@
     <definedName name="x">Sheet1!$B$2</definedName>
     <definedName name="y">Sheet1!$F$2</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Inputs</t>
   </si>
@@ -50,9 +55,6 @@
     <t>b</t>
   </si>
   <si>
-    <t>2.12345*x</t>
-  </si>
-  <si>
     <t>~b</t>
   </si>
   <si>
@@ -63,13 +65,19 @@
   </si>
   <si>
     <t>Context</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>2..1*x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +184,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -222,7 +238,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,9 +270,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,6 +305,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -463,37 +481,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -502,14 +520,14 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F2" s="4">
-        <f>x*2.12345</f>
+        <f>x*2.1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -518,14 +536,14 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="4" t="b">
         <f>IF(b, FALSE, TRUE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -534,12 +552,21 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5" t="str">
         <f>LOWER(s)</f>
         <v/>
       </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>0.12</v>
+      </c>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -548,24 +575,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>Sheet1!B5+100</f>
+        <v>100.12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
test for excel wrapper
</commit_message>
<xml_diff>
--- a/src/excel_wrapper/test/excel_wrapper_test.xlsx
+++ b/src/excel_wrapper/test/excel_wrapper_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PLUGIN-1.x\excel_wrapper1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\excel_wrapper_meta\excel_wrapper\src\excel_wrapper\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Inputs</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>2..1*x</t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +518,9 @@
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3">
+        <v>12</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
@@ -524,14 +529,16 @@
       </c>
       <c r="F2" s="4">
         <f>x*2.1</f>
-        <v>0</v>
+        <v>25.200000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
@@ -540,14 +547,16 @@
       </c>
       <c r="F3" s="4" t="b">
         <f>IF(b, FALSE, TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
@@ -556,7 +565,7 @@
       </c>
       <c r="F4" s="5" t="str">
         <f>LOWER(s)</f>
-        <v/>
+        <v>hello</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>